<commit_message>
Fix a few typos.
</commit_message>
<xml_diff>
--- a/misc/AcroMath.xlsx
+++ b/misc/AcroMath.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rnolan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rnolan/Dropbox/DPhil/phdthesis/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D95CC0ED-2C57-C84A-B03C-A1B0EB8D9A76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BC79C603-1C9D-C649-8FEC-0064A078E13F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="-29740" windowWidth="28800" windowHeight="50740" xr2:uid="{64105B43-CF8D-6940-AC69-9D1135036A2A}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>GaAsP</t>
   </si>
   <si>
-    <t>Gallium arsenide phosphide</t>
-  </si>
-  <si>
     <t>TIRF</t>
   </si>
   <si>
@@ -502,9 +499,6 @@
     <t>Cluster of Differentiation 4</t>
   </si>
   <si>
-    <t>CCR</t>
-  </si>
-  <si>
     <t>C-Chemokyne Receptor 5</t>
   </si>
   <si>
@@ -541,9 +535,6 @@
     <t>ALEX</t>
   </si>
   <si>
-    <t>Alternating Laser Excitation</t>
-  </si>
-  <si>
     <t>JR-FL</t>
   </si>
   <si>
@@ -575,6 +566,15 @@
   </si>
   <si>
     <t>Forster Resonance Energy Transfer</t>
+  </si>
+  <si>
+    <t>CCR5</t>
+  </si>
+  <si>
+    <t>Gallium Arsenide Phosphide</t>
+  </si>
+  <si>
+    <t>Alternating Laser EXcitation</t>
   </si>
 </sst>
 </file>
@@ -929,14 +929,14 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1067,127 +1067,127 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
         <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
         <v>122</v>
-      </c>
-      <c r="B30" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" t="s">
         <v>124</v>
-      </c>
-      <c r="B31" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" t="s">
         <v>126</v>
-      </c>
-      <c r="B32" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1200,130 +1200,130 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
         <v>128</v>
-      </c>
-      <c r="B34" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" t="s">
         <v>130</v>
-      </c>
-      <c r="B35" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
         <v>154</v>
-      </c>
-      <c r="B36" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" t="s">
         <v>156</v>
-      </c>
-      <c r="B37" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B40" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>169</v>
+      </c>
+      <c r="B45" t="s">
         <v>172</v>
-      </c>
-      <c r="B45" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B49" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1347,354 +1347,354 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
         <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
         <v>80</v>
-      </c>
-      <c r="B12" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
         <v>82</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
         <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
         <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
         <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
         <v>92</v>
-      </c>
-      <c r="B19" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
         <v>94</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
         <v>96</v>
-      </c>
-      <c r="B21" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
         <v>98</v>
-      </c>
-      <c r="B22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
         <v>116</v>
-      </c>
-      <c r="B24" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" t="s">
         <v>102</v>
-      </c>
-      <c r="B25" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
         <v>105</v>
-      </c>
-      <c r="B27" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
         <v>107</v>
-      </c>
-      <c r="B28" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
         <v>109</v>
-      </c>
-      <c r="B29" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
         <v>111</v>
-      </c>
-      <c r="B30" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" t="s">
         <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" t="s">
         <v>118</v>
-      </c>
-      <c r="B33" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" t="s">
         <v>120</v>
-      </c>
-      <c r="B34" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" t="s">
         <v>132</v>
-      </c>
-      <c r="B35" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" t="s">
         <v>134</v>
-      </c>
-      <c r="B36" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
         <v>136</v>
-      </c>
-      <c r="B37" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" t="s">
         <v>138</v>
-      </c>
-      <c r="B38" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" t="s">
         <v>141</v>
-      </c>
-      <c r="B39" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" t="s">
         <v>143</v>
-      </c>
-      <c r="B40" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" t="s">
         <v>145</v>
-      </c>
-      <c r="B41" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" t="s">
         <v>147</v>
-      </c>
-      <c r="B42" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" t="s">
         <v>149</v>
-      </c>
-      <c r="B43" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" t="s">
         <v>152</v>
-      </c>
-      <c r="B44" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>